<commit_message>
Graph utils deleted and Excel file updated
</commit_message>
<xml_diff>
--- a/Resultados experimentos.xlsx
+++ b/Resultados experimentos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanp\dev\graphs-tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30507029-C458-43F4-9108-7509C2276FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8390BD2F-188C-416A-A735-1E6B222F943F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,24 +25,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Cantidad de caracteres original</t>
-  </si>
-  <si>
-    <t>Cantidad de consultas</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Experimento no.</t>
   </si>
   <si>
-    <t>Segundos en escenario 1</t>
+    <t>Cantidad de vértices</t>
   </si>
   <si>
-    <t>Segundos en escenario 2</t>
+    <t>Algoritmo no.</t>
   </si>
   <si>
-    <t>No alcanzamos a probar los escenarios porque se estaba demorando demasiado</t>
+    <t>Cantidad de vértices hayados en la solución</t>
+  </si>
+  <si>
+    <t>Tiempo</t>
   </si>
 </sst>
 </file>
@@ -89,12 +86,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -104,6 +104,7 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -155,14 +156,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1B7706D5-DB7F-47FB-87AC-F24EEDBE857A}" name="Tabla1" displayName="Tabla1" ref="B2:F14" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="B2:F14" xr:uid="{1B7706D5-DB7F-47FB-87AC-F24EEDBE857A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1B7706D5-DB7F-47FB-87AC-F24EEDBE857A}" name="Tabla1" displayName="Tabla1" ref="F2:J23" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="F2:J23" xr:uid="{1B7706D5-DB7F-47FB-87AC-F24EEDBE857A}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{D1EB1912-16EB-40FE-9317-12FB891E6113}" name="Experimento no." dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{C527D2CB-C0DA-4BEA-AA5A-99F93E8DE8CA}" name="Cantidad de caracteres original" dataDxfId="3" dataCellStyle="Moneda"/>
-    <tableColumn id="3" xr3:uid="{AD94BA08-6D83-4BAE-86CF-6B27089D8901}" name="Cantidad de consultas" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{1D76434B-9678-4ED0-9B58-B0EE00F76004}" name="Segundos en escenario 1" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{310FA9E9-9F8A-45C4-93CC-7A538C43B1C2}" name="Segundos en escenario 2" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{C527D2CB-C0DA-4BEA-AA5A-99F93E8DE8CA}" name="Algoritmo no." dataDxfId="3" dataCellStyle="Moneda"/>
+    <tableColumn id="3" xr3:uid="{AD94BA08-6D83-4BAE-86CF-6B27089D8901}" name="Cantidad de vértices" dataDxfId="0" dataCellStyle="Moneda"/>
+    <tableColumn id="4" xr3:uid="{1D76434B-9678-4ED0-9B58-B0EE00F76004}" name="Cantidad de vértices hayados en la solución" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{310FA9E9-9F8A-45C4-93CC-7A538C43B1C2}" name="Tiempo" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -431,203 +432,316 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F17"/>
+  <dimension ref="F2:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.140625" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="44.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="1">
+      <c r="J2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="2">
-        <v>100000</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3">
+        <v>100</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3">
         <v>1000</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="1">
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F5" s="1">
+        <v>3</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3">
+        <v>10000</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F6" s="1">
+        <v>4</v>
+      </c>
+      <c r="G6" s="2">
         <v>2</v>
       </c>
-      <c r="C4" s="2">
-        <v>100000</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="H6" s="3">
+        <v>100</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F7" s="1">
+        <v>5</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1000</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F8" s="1">
+        <v>6</v>
+      </c>
+      <c r="G8" s="2">
+        <v>2</v>
+      </c>
+      <c r="H8" s="3">
         <v>10000</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="1">
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F9" s="1">
+        <v>7</v>
+      </c>
+      <c r="G9" s="2">
         <v>3</v>
       </c>
-      <c r="C5" s="2">
-        <v>100000</v>
-      </c>
-      <c r="D5" s="1">
-        <v>100000</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="1">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2">
-        <v>100000</v>
-      </c>
-      <c r="D6" s="1">
-        <v>1000000</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="1">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1000000</v>
-      </c>
-      <c r="D7" s="1">
+      <c r="H9" s="3">
+        <v>100</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F10" s="1">
+        <v>8</v>
+      </c>
+      <c r="G10" s="2">
+        <v>3</v>
+      </c>
+      <c r="H10" s="3">
         <v>1000</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="1">
-        <v>6</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1000000</v>
-      </c>
-      <c r="D8" s="1">
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F11" s="1">
+        <v>9</v>
+      </c>
+      <c r="G11" s="2">
+        <v>3</v>
+      </c>
+      <c r="H11" s="3">
         <v>10000</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="1">
-        <v>7</v>
-      </c>
-      <c r="C9" s="2">
-        <v>1000000</v>
-      </c>
-      <c r="D9" s="1">
-        <v>100000</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="1">
-        <v>8</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1000000</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1000000</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="1">
-        <v>9</v>
-      </c>
-      <c r="C11" s="2">
-        <v>10000000</v>
-      </c>
-      <c r="D11" s="1">
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F12" s="1">
+        <v>10</v>
+      </c>
+      <c r="G12" s="2">
+        <v>4</v>
+      </c>
+      <c r="H12" s="3">
+        <v>100</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F13" s="1">
+        <v>11</v>
+      </c>
+      <c r="G13" s="2">
+        <v>4</v>
+      </c>
+      <c r="H13" s="3">
+        <v>100</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F14" s="1">
+        <v>12</v>
+      </c>
+      <c r="G14" s="2">
+        <v>4</v>
+      </c>
+      <c r="H14" s="3">
+        <v>100</v>
+      </c>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F15" s="1">
+        <v>13</v>
+      </c>
+      <c r="G15" s="2">
+        <v>4</v>
+      </c>
+      <c r="H15" s="3">
+        <v>100</v>
+      </c>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F16" s="1">
+        <v>14</v>
+      </c>
+      <c r="G16" s="2">
+        <v>4</v>
+      </c>
+      <c r="H16" s="3">
         <v>1000</v>
       </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="1">
-        <v>10</v>
-      </c>
-      <c r="C12" s="2">
-        <v>10000000</v>
-      </c>
-      <c r="D12" s="1">
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F17" s="1">
+        <v>15</v>
+      </c>
+      <c r="G17" s="2">
+        <v>4</v>
+      </c>
+      <c r="H17" s="3">
+        <v>1000</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F18" s="1">
+        <v>16</v>
+      </c>
+      <c r="G18" s="2">
+        <v>4</v>
+      </c>
+      <c r="H18" s="3">
+        <v>1000</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F19" s="1">
+        <v>17</v>
+      </c>
+      <c r="G19" s="2">
+        <v>4</v>
+      </c>
+      <c r="H19" s="3">
+        <v>1000</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F20" s="1">
+        <v>18</v>
+      </c>
+      <c r="G20" s="2">
+        <v>4</v>
+      </c>
+      <c r="H20" s="3">
         <v>10000</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="1">
-        <v>11</v>
-      </c>
-      <c r="C13" s="2">
-        <v>10000000</v>
-      </c>
-      <c r="D13" s="1">
-        <v>100000</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="1">
-        <v>12</v>
-      </c>
-      <c r="C14" s="2">
-        <v>10000000</v>
-      </c>
-      <c r="D14" s="1">
-        <v>1000000</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>5</v>
-      </c>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F21" s="1">
+        <v>19</v>
+      </c>
+      <c r="G21" s="2">
+        <v>4</v>
+      </c>
+      <c r="H21" s="3">
+        <v>10000</v>
+      </c>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F22" s="1">
+        <v>20</v>
+      </c>
+      <c r="G22" s="2">
+        <v>4</v>
+      </c>
+      <c r="H22" s="3">
+        <v>10000</v>
+      </c>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F23" s="1">
+        <v>21</v>
+      </c>
+      <c r="G23" s="2">
+        <v>4</v>
+      </c>
+      <c r="H23" s="3">
+        <v>10000</v>
+      </c>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>